<commit_message>
Enemies may drop bandages now!
</commit_message>
<xml_diff>
--- a/gun informations.xlsx
+++ b/gun informations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\multiplayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4782AF-20BA-4B15-B6E3-7B3A36ABDC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751D0458-9675-49DF-9E30-FC315FA0DAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-310" yWindow="3360" windowWidth="38400" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1060" windowWidth="38400" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -327,10 +327,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>absorbed damage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>reduced DPR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -340,6 +336,10 @@
   </si>
   <si>
     <t>pierce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>absorbed DPR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -962,7 +962,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -998,7 +998,7 @@
         <v>46</v>
       </c>
       <c r="T1" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.45">
@@ -1055,10 +1055,10 @@
         <v>53</v>
       </c>
       <c r="T2" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U2" s="34" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="Y2" t="s">
         <v>0</v>
@@ -1119,10 +1119,10 @@
       </c>
       <c r="S3" s="11"/>
       <c r="T3" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
@@ -2622,7 +2622,7 @@
       <c r="C29" s="11">
         <v>0</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="11">
         <v>1</v>
       </c>
       <c r="E29" s="11">

</xml_diff>